<commit_message>
move UART header back away from case edge
</commit_message>
<xml_diff>
--- a/Hardware/stm32-pi_full/stm32 v1.1 working BoM/JLCSMT_Sample_CPL1.xlsx
+++ b/Hardware/stm32-pi_full/stm32 v1.1 working BoM/JLCSMT_Sample_CPL1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d4/Documents/github/emonSTM32-db/Hardware/stm32-pi_full/stm32 v1.0 working BoM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d4/Documents/github/emonSTM32-db/Hardware/stm32-pi_full/stm32 v1.1 working BoM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D795BF-1218-EB45-9357-3D18C2866D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35637CAD-BE2F-0B44-BCF1-D750DF302F1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <dimension ref="A1:E182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1688,10 +1688,10 @@
         <v>45</v>
       </c>
       <c r="B41" s="3">
-        <v>13.44</v>
+        <v>13.28</v>
       </c>
       <c r="C41" s="3">
-        <v>8.82</v>
+        <v>11.96</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>

</xml_diff>